<commit_message>
GDE-8270: pushed updated datasets
</commit_message>
<xml_diff>
--- a/DataSet/Integration_DataSet/TL/FXRates_GSFile/EU/TL_FX_04_Files/TL_Transformed_Data_FXRates0.xlsx
+++ b/DataSet/Integration_DataSet/TL/FXRates_GSFile/EU/TL_FX_04_Files/TL_Transformed_Data_FXRates0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\TL\FXRates_GSFile\EU\TL_FX_01_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Evergreen\fms_cba\DataSet\Integration_DataSet\TL\FXRates_GSFile\EU\TL_FX_04_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB65848-E8B1-45C0-88F1-C4F420A7A828}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA1FAEA-1AA6-4A8D-8477-263398F8B992}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10590" yWindow="555" windowWidth="20025" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transformed_FXRates" sheetId="1" r:id="rId1"/>
@@ -343,13 +343,13 @@
     <t>9.0574</t>
   </si>
   <si>
-    <t>2020-04-25</t>
-  </si>
-  <si>
-    <t>3.55</t>
-  </si>
-  <si>
     <t>1.11</t>
+  </si>
+  <si>
+    <t>3.21</t>
+  </si>
+  <si>
+    <t>2021-10-28</t>
   </si>
 </sst>
 </file>
@@ -745,7 +745,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -823,7 +823,7 @@
         <v>17</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I2" t="s">
         <v>18</v>
@@ -858,7 +858,7 @@
         <v>25</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I3" t="s">
         <v>18</v>
@@ -893,7 +893,7 @@
         <v>30</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I4" t="s">
         <v>18</v>
@@ -928,7 +928,7 @@
         <v>35</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I5" t="s">
         <v>18</v>
@@ -963,7 +963,7 @@
         <v>40</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I6" t="s">
         <v>18</v>
@@ -998,7 +998,7 @@
         <v>45</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I7" t="s">
         <v>18</v>
@@ -1033,7 +1033,7 @@
         <v>48</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I8" t="s">
         <v>18</v>
@@ -1068,7 +1068,7 @@
         <v>53</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I9" t="s">
         <v>18</v>
@@ -1103,7 +1103,7 @@
         <v>58</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I10" t="s">
         <v>18</v>
@@ -1138,7 +1138,7 @@
         <v>63</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I11" t="s">
         <v>18</v>
@@ -1173,7 +1173,7 @@
         <v>68</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I12" t="s">
         <v>18</v>
@@ -1208,7 +1208,7 @@
         <v>73</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I13" t="s">
         <v>18</v>
@@ -1243,7 +1243,7 @@
         <v>78</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I14" t="s">
         <v>18</v>
@@ -1272,13 +1272,13 @@
         <v>81</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G15" t="s">
         <v>82</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I15" t="s">
         <v>18</v>
@@ -1313,7 +1313,7 @@
         <v>87</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I16" t="s">
         <v>18</v>
@@ -1348,7 +1348,7 @@
         <v>87</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I17" t="s">
         <v>18</v>
@@ -1383,7 +1383,7 @@
         <v>96</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I18" t="s">
         <v>18</v>
@@ -1418,7 +1418,7 @@
         <v>101</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I19" t="s">
         <v>18</v>
@@ -1453,7 +1453,7 @@
         <v>106</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I20" t="s">
         <v>18</v>

</xml_diff>